<commit_message>
[20191113] - Aggregation Assignment Added
</commit_message>
<xml_diff>
--- a/assignment_overview.xlsx
+++ b/assignment_overview.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20">
   <si>
     <t>WinRT Assignments</t>
   </si>
@@ -31,13 +31,49 @@
     <t>Uploaded</t>
   </si>
   <si>
+    <t>Essay</t>
+  </si>
+  <si>
     <t>Pending</t>
   </si>
   <si>
+    <t>First Application</t>
+  </si>
+  <si>
+    <t>Hello World</t>
+  </si>
+  <si>
     <t>Rejected</t>
   </si>
   <si>
+    <t>MessageBox</t>
+  </si>
+  <si>
     <t>Accepted</t>
+  </si>
+  <si>
+    <t>SplashScreen</t>
+  </si>
+  <si>
+    <t>Pledge</t>
+  </si>
+  <si>
+    <t>ColorChange</t>
+  </si>
+  <si>
+    <t>Stripes</t>
+  </si>
+  <si>
+    <t>DLL &amp; DLL Client</t>
+  </si>
+  <si>
+    <t>MultiThreading</t>
+  </si>
+  <si>
+    <t>ClassFactory</t>
+  </si>
+  <si>
+    <t>Containment</t>
   </si>
 </sst>
 </file>
@@ -45,12 +81,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,26 +125,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -122,6 +151,75 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -129,107 +227,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -272,12 +301,120 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -290,6 +427,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -302,7 +445,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -320,133 +469,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -471,6 +500,15 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -531,11 +569,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -557,166 +601,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="36" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1060,7 +1089,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="C2:I20"/>
+  <dimension ref="C2:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:F2"/>
@@ -1103,9 +1132,11 @@
       <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="H4" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I4" s="10"/>
     </row>
@@ -1117,7 +1148,9 @@
       <c r="E5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="H5" s="7" t="s">
         <v>4</v>
       </c>
@@ -1131,9 +1164,11 @@
       <c r="E6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="H6" s="7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I6" s="12"/>
     </row>
@@ -1145,9 +1180,11 @@
       <c r="E7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="H7" s="7" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I7" s="13"/>
     </row>
@@ -1159,7 +1196,9 @@
       <c r="E8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="3:6">
       <c r="C9" s="4">
@@ -1167,9 +1206,11 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="3:6">
       <c r="C10" s="4">
@@ -1179,7 +1220,9 @@
       <c r="E10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="3:6">
       <c r="C11" s="4">
@@ -1189,7 +1232,9 @@
       <c r="E11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="3:6">
       <c r="C12" s="4">
@@ -1199,7 +1244,9 @@
       <c r="E12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="3:6">
       <c r="C13" s="4"/>
@@ -1269,17 +1316,81 @@
       <c r="E19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="6"/>
+      <c r="F19" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="20" spans="3:6">
-      <c r="C20" s="9">
+      <c r="C20" s="4">
         <v>11</v>
       </c>
-      <c r="D20" s="9"/>
+      <c r="D20" s="4"/>
       <c r="E20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="9"/>
+      <c r="F20" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6">
+      <c r="C21" s="9">
+        <v>12</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6">
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="3:6">
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="3:6">
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="3:6">
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="3:6">
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="3:6">
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="3:6">
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="3:6">
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>